<commit_message>
Add another example data sheet
</commit_message>
<xml_diff>
--- a/excel_test_data.xlsx
+++ b/excel_test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitlab\GGRD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6484643-60E1-466A-8CDD-28832AA95492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FD1C95-28DC-4CF8-9BFE-68F229122D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>purge</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +46,50 @@
   </si>
   <si>
     <t>NH3_purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[B2] start of ill-format excel file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A8] second data appearance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A13] contiguous column data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[B13] contiguous column data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[C13] contiguous column data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A16] contiguous row data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A17] contiguous row data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A18] contiguous row data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[A2] jumping column data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[G22] jumping column data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[H22] jumping column data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16ED2F1-746D-473C-8DDE-7F69B695D8C7}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -553,4 +598,67 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F9B266-1E83-463B-8B28-4F5777F3C84D}">
+  <dimension ref="A2:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.45" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>